<commit_message>
auto filter for Excel
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_020_b-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_020_b-xlsx.w3mi.data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\moldab\Desktop\abapgit save\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{AF308ECD-8325-4801-903C-2C463A60ACAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" tabRatio="703" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" tabRatio="703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelTable" sheetId="4" r:id="rId1"/>
@@ -17,12 +18,13 @@
     <sheet name="PrintArea ('8' rows)" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'PrintArea (''8'' rows)'!$B$3:$C$3</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'PrintArea (''8'' rows)'!$A$1:$E$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'PrintArea (''8'' rows)'!$2:$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -87,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -936,7 +938,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[ZXXT_02_EXCEL_B.XLSX]Pivot based on ExcelTable!PivotTable1</c:name>
+    <c:name>[ZXXT_DEMO_020_B.XLSX]Pivot based on ExcelTable!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1975,7 +1977,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1994,7 +2002,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44221.34225775463" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44476.369375231479" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -2028,7 +2036,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisPage" compact="0" outline="0" showAll="0">
@@ -2125,19 +2133,22 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E6" totalsRowCount="1" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
-  <autoFilter ref="A4:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A4:E6" totalsRowCount="1" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="A4:E5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Caption" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" name="Group" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" name="Date" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="SUM 1" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="SUM 2" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Caption" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Date" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SUM 1" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SUM 2" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2439,10 +2450,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2518,7 +2529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2581,10 +2592,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2643,12 +2654,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B3:C3" xr:uid="{41244A09-8ED0-4A14-B973-11EA4FBF1781}"/>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E4" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>NOW()-3</formula1>
       <formula2>NOW()+3</formula2>
     </dataValidation>

</xml_diff>